<commit_message>
Update results file with execution times
</commit_message>
<xml_diff>
--- a/experiment_results.xlsx
+++ b/experiment_results.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KYRIAKOS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF033275-2157-423D-8287-CECF7DFEB5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E194FEA-5550-4B5A-B090-C51B496447E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{BF746F91-F0B7-4EE2-B6D7-959D345E6735}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BF746F91-F0B7-4EE2-B6D7-959D345E6735}"/>
   </bookViews>
   <sheets>
-    <sheet name="5 Nodes" sheetId="1" r:id="rId1"/>
-    <sheet name="10 Nodes" sheetId="2" r:id="rId2"/>
-    <sheet name="Zusammen" sheetId="3" r:id="rId3"/>
+    <sheet name="Execution Times" sheetId="4" r:id="rId1"/>
+    <sheet name="5 Nodes" sheetId="1" r:id="rId2"/>
+    <sheet name="10 Nodes" sheetId="2" r:id="rId3"/>
+    <sheet name="Zusammen" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
   <si>
     <t>Throughput</t>
   </si>
@@ -112,6 +113,18 @@
   <si>
     <t>10 Nodes</t>
   </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>5 nodes</t>
+  </si>
+  <si>
+    <t>10 nodes</t>
+  </si>
+  <si>
+    <t>time in seconds</t>
+  </si>
 </sst>
 </file>
 
@@ -132,12 +145,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -152,8 +171,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4580,6 +4603,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77429401-50E9-4791-9E5B-8F720A661323}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>5</v>
+      </c>
+      <c r="D1">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1049</v>
+      </c>
+      <c r="C2">
+        <v>503</v>
+      </c>
+      <c r="D2">
+        <v>642</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>11299</v>
+      </c>
+      <c r="C3">
+        <v>4330</v>
+      </c>
+      <c r="D3">
+        <v>3165</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1934</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1088</v>
+      </c>
+      <c r="D4" s="1">
+        <v>760</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>32206</v>
+      </c>
+      <c r="C5" s="1">
+        <v>16321</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4748</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE2D0BC-CC51-4CB3-9D3D-7A3548EC3EDC}">
   <dimension ref="A1:N24"/>
   <sheetViews>
@@ -4917,7 +5047,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70C8343-6A4F-4E0E-ACE8-3B4A3478D678}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -5293,11 +5423,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E81ED0-1DB3-4EDC-9642-701611F8B179}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>

</xml_diff>